<commit_message>
Updated two risk evaluations. Risk impact cant go down
</commit_message>
<xml_diff>
--- a/Risk Assessment/Risk Assesment v01.xlsx
+++ b/Risk Assessment/Risk Assesment v01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d57b30c47c6b917/Daniel/School/Saxion/Leerjaar 4a/Process and Safety/Repositories/PS_diagrams/Risk Assessment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markh\Desktop\Local repo\PS_diagrams-1\Risk Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{12CA9A15-C177-439D-A915-7CFA9C59FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08D53D4B-85DC-4B60-A6D7-514BDAB95594}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7142ADB-A8F4-4B75-A4C2-7C840D42D31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B58E22B4-07E1-4452-ADE0-1C38FF088435}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B58E22B4-07E1-4452-ADE0-1C38FF088435}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,10 +538,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -845,7 +841,7 @@
   <dimension ref="A1:BI456"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1079,10 @@
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>17</v>
@@ -1125,10 +1121,10 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I8" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="24" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Rmoved example in RA
</commit_message>
<xml_diff>
--- a/Risk Assessment/Risk Assesment v01.xlsx
+++ b/Risk Assessment/Risk Assesment v01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markh\Desktop\Local repo\PS_diagrams-1\Risk Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7142ADB-A8F4-4B75-A4C2-7C840D42D31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7519B38-4628-4B3A-BF75-10E471EB3E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B58E22B4-07E1-4452-ADE0-1C38FF088435}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>Risk/ hazard description</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Likely</t>
   </si>
   <si>
-    <t>Cutting hazard when operating knife in cooking process</t>
-  </si>
-  <si>
-    <t>Operator training; Frequent equipment maintenance</t>
-  </si>
-  <si>
     <t>Mechanical</t>
   </si>
   <si>
@@ -168,13 +162,25 @@
   </si>
   <si>
     <t>Operator training; Light curtain</t>
+  </si>
+  <si>
+    <t>Keep monitoring</t>
+  </si>
+  <si>
+    <t>Measures advised</t>
+  </si>
+  <si>
+    <t>Take measures now</t>
+  </si>
+  <si>
+    <t>Legend:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,14 +220,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -376,37 +374,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -423,13 +390,81 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF0000FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF0000FF"/>
       </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF0000FF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -442,7 +477,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -465,29 +500,31 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -523,8 +560,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFF9393"/>
-      <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -841,7 +878,7 @@
   <dimension ref="A1:BI456"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,54 +937,54 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="26">
-        <v>4</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="26" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="27">
-        <v>2</v>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
       </c>
       <c r="L3" s="17"/>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -958,16 +995,16 @@
       <c r="I4" s="6">
         <v>1</v>
       </c>
-      <c r="L4" s="31" t="s">
+      <c r="L4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="29" t="s">
+      <c r="O4" s="25" t="s">
         <v>12</v>
       </c>
       <c r="P4" s="30" t="s">
@@ -977,7 +1014,7 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -989,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -1000,7 +1037,7 @@
       <c r="I5" s="6">
         <v>1</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="23" t="s">
         <v>14</v>
       </c>
       <c r="M5" s="7">
@@ -1025,24 +1062,24 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="L6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="23" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="7">
@@ -1061,7 +1098,7 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1073,7 +1110,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -1084,7 +1121,7 @@
       <c r="I7" s="6">
         <v>2</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="M7" s="8">
@@ -1102,31 +1139,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="6">
-        <v>2</v>
-      </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="M8" s="8">
@@ -1147,26 +1160,29 @@
       <c r="B9" s="5"/>
       <c r="I9" s="6"/>
       <c r="L9" s="18"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
       <c r="P9" s="20"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="I10" s="6"/>
-      <c r="L10" s="23" t="s">
+      <c r="L10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="P10" s="20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1174,73 +1190,84 @@
       <c r="B11" s="5"/>
       <c r="I11" s="6"/>
       <c r="L11" s="18"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
       <c r="P11" s="20"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="I12" s="6"/>
-      <c r="L12" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="20"/>
+      <c r="L12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="I13" s="6"/>
       <c r="L13" s="18"/>
-      <c r="M13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P13" s="20"/>
+      <c r="M13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="33" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="I14" s="6"/>
       <c r="L14" s="18"/>
-      <c r="M14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P14" s="20"/>
+      <c r="M14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="I15" s="6"/>
       <c r="L15" s="18"/>
-      <c r="M15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" s="20"/>
+      <c r="M15" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="35" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -1249,7 +1276,7 @@
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
-      <c r="P16" s="22"/>
+      <c r="P16" s="36"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -3118,7 +3145,7 @@
   <mergeCells count="1">
     <mergeCell ref="M3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E248 I3:I288 F4:F8">
+  <conditionalFormatting sqref="E9:E248 E3:F7 I9:I288 I3:I7">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>5</formula>
       <formula>7</formula>

</xml_diff>

<commit_message>
Added compressed air failure
</commit_message>
<xml_diff>
--- a/Risk Assessment/Risk Assesment v01.xlsx
+++ b/Risk Assessment/Risk Assesment v01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markh\Desktop\Local repo\PS_diagrams-1\Risk Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7519B38-4628-4B3A-BF75-10E471EB3E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11760ACF-E936-4F3E-871C-EFD4E92B93D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B58E22B4-07E1-4452-ADE0-1C38FF088435}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Risk/ hazard description</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>Legend:</t>
+  </si>
+  <si>
+    <t>Compressed air explosion</t>
+  </si>
+  <si>
+    <t>Unlikley</t>
+  </si>
+  <si>
+    <t>Regular preventative maintenance</t>
   </si>
 </sst>
 </file>
@@ -288,19 +297,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF0000FF"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF0000FF"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -468,6 +464,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -477,37 +482,43 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -515,16 +526,30 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -877,8 +902,8 @@
   </sheetPr>
   <dimension ref="A1:BI456"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,11 +912,11 @@
     <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="36" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="19" width="18.42578125" style="2" customWidth="1"/>
     <col min="20" max="37" width="15.140625" style="2" customWidth="1"/>
@@ -902,42 +927,42 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
@@ -946,7 +971,7 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="36">
         <v>3</v>
       </c>
       <c r="F3" t="s">
@@ -958,20 +983,20 @@
       <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="42">
         <v>1</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="27" t="s">
+      <c r="L3" s="14"/>
+      <c r="M3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="29"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="32"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C4" t="s">
@@ -980,7 +1005,7 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="41">
         <v>2</v>
       </c>
       <c r="F4" t="s">
@@ -992,79 +1017,79 @@
       <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="42">
         <v>1</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
-        <v>37</v>
+      <c r="A5" s="35"/>
+      <c r="B5" s="34" t="s">
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="E5" s="41">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="42">
+        <v>2</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <v>2</v>
+      </c>
+      <c r="O5" s="7">
+        <v>3</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="6">
-        <v>1</v>
-      </c>
-      <c r="L5" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>2</v>
-      </c>
-      <c r="O5" s="8">
-        <v>3</v>
-      </c>
-      <c r="P5" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
+      <c r="E6" s="41">
         <v>3</v>
       </c>
       <c r="F6" t="s">
@@ -1074,40 +1099,40 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="6">
+        <v>10</v>
+      </c>
+      <c r="I6" s="42">
+        <v>1</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="6">
         <v>2</v>
       </c>
-      <c r="L6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="7">
-        <v>2</v>
-      </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>3</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>4</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
-        <v>40</v>
+      <c r="A7" s="35"/>
+      <c r="B7" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7">
-        <v>3</v>
+      <c r="E7" s="36">
+        <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
@@ -1118,2034 +1143,2064 @@
       <c r="H7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="42">
         <v>2</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>3</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>4</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <v>5</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="L8" s="23" t="s">
+      <c r="A8" s="35"/>
+      <c r="B8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="36">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="42">
+        <v>2</v>
+      </c>
+      <c r="L8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="7">
         <v>4</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <v>5</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="10">
         <v>6</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="20"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="34"/>
+      <c r="I9" s="39"/>
+      <c r="L9" s="15"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="L10" s="22" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="34"/>
+      <c r="I10" s="39"/>
+      <c r="L10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="N10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P10" s="20" t="s">
+      <c r="P10" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="20"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="34"/>
+      <c r="I11" s="39"/>
+      <c r="L11" s="15"/>
+      <c r="P11" s="17"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="L12" s="22" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" s="34"/>
+      <c r="I12" s="39"/>
+      <c r="L12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="31" t="s">
+      <c r="M12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="31" t="s">
+      <c r="N12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="31" t="s">
+      <c r="O12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="32" t="s">
+      <c r="P12" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="31" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="34"/>
+      <c r="I13" s="39"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O13" s="31" t="s">
+      <c r="O13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="33" t="s">
+      <c r="P13" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="31" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="34"/>
+      <c r="I14" s="39"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="31" t="s">
+      <c r="N14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="31" t="s">
+      <c r="O14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P14" s="34" t="s">
+      <c r="P14" s="27" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="31" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="34"/>
+      <c r="I15" s="39"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N15" s="31" t="s">
+      <c r="N15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O15" s="31" t="s">
+      <c r="O15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="36"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="34"/>
+      <c r="I16" s="39"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="29"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="34"/>
+      <c r="I17" s="39"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="34"/>
+      <c r="I18" s="39"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="34"/>
+      <c r="I19" s="39"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="34"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="34"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="34"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="34"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="34"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="34"/>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="34"/>
+      <c r="I26" s="39"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="34"/>
+      <c r="I27" s="39"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="I28" s="6"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="34"/>
+      <c r="I28" s="39"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="I29" s="6"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="34"/>
+      <c r="I29" s="39"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="I30" s="6"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="34"/>
+      <c r="I30" s="39"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
-      <c r="I31" s="6"/>
+      <c r="I31" s="39"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
-      <c r="I32" s="6"/>
+      <c r="I32" s="39"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
-      <c r="I33" s="6"/>
+      <c r="I33" s="39"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
-      <c r="I34" s="6"/>
+      <c r="I34" s="39"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
-      <c r="I35" s="6"/>
+      <c r="I35" s="39"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
-      <c r="I36" s="6"/>
+      <c r="I36" s="39"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
-      <c r="I37" s="6"/>
+      <c r="I37" s="39"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
-      <c r="I38" s="6"/>
+      <c r="I38" s="39"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
-      <c r="I39" s="6"/>
+      <c r="I39" s="39"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
-      <c r="I40" s="6"/>
+      <c r="I40" s="39"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
-      <c r="I41" s="6"/>
+      <c r="I41" s="39"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
-      <c r="I42" s="6"/>
+      <c r="I42" s="39"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
-      <c r="I43" s="6"/>
+      <c r="I43" s="39"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
-      <c r="I44" s="6"/>
+      <c r="I44" s="39"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
-      <c r="I45" s="6"/>
+      <c r="I45" s="39"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
-      <c r="I46" s="6"/>
+      <c r="I46" s="39"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
-      <c r="I47" s="6"/>
+      <c r="I47" s="39"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
-      <c r="I48" s="6"/>
+      <c r="I48" s="39"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
-      <c r="I49" s="6"/>
+      <c r="I49" s="39"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="5"/>
-      <c r="I50" s="6"/>
+      <c r="I50" s="39"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
-      <c r="I51" s="6"/>
+      <c r="I51" s="39"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="5"/>
-      <c r="I52" s="6"/>
+      <c r="I52" s="39"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="5"/>
-      <c r="I53" s="6"/>
+      <c r="I53" s="39"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="5"/>
-      <c r="I54" s="6"/>
+      <c r="I54" s="39"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
-      <c r="I55" s="6"/>
+      <c r="I55" s="39"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="5"/>
-      <c r="I56" s="6"/>
+      <c r="I56" s="39"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="5"/>
-      <c r="I57" s="6"/>
+      <c r="I57" s="39"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="5"/>
-      <c r="I58" s="6"/>
+      <c r="I58" s="39"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="5"/>
-      <c r="I59" s="6"/>
+      <c r="I59" s="39"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="5"/>
-      <c r="I60" s="6"/>
+      <c r="I60" s="39"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
-      <c r="I61" s="6"/>
+      <c r="I61" s="39"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="5"/>
-      <c r="I62" s="6"/>
+      <c r="I62" s="39"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="5"/>
-      <c r="I63" s="6"/>
+      <c r="I63" s="39"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
-      <c r="I64" s="6"/>
+      <c r="I64" s="39"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
-      <c r="I65" s="6"/>
+      <c r="I65" s="39"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="5"/>
-      <c r="I66" s="6"/>
+      <c r="I66" s="39"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="5"/>
-      <c r="I67" s="6"/>
+      <c r="I67" s="39"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="5"/>
-      <c r="I68" s="6"/>
+      <c r="I68" s="39"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="5"/>
-      <c r="I69" s="6"/>
+      <c r="I69" s="39"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="5"/>
-      <c r="I70" s="6"/>
+      <c r="I70" s="39"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
-      <c r="I71" s="6"/>
+      <c r="I71" s="39"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="5"/>
-      <c r="I72" s="6"/>
+      <c r="I72" s="39"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="5"/>
-      <c r="I73" s="6"/>
+      <c r="I73" s="39"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="5"/>
-      <c r="I74" s="6"/>
+      <c r="I74" s="39"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="5"/>
-      <c r="I75" s="6"/>
+      <c r="I75" s="39"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="5"/>
-      <c r="I76" s="6"/>
+      <c r="I76" s="39"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
-      <c r="I77" s="6"/>
+      <c r="I77" s="39"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="5"/>
-      <c r="I78" s="6"/>
+      <c r="I78" s="39"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="5"/>
-      <c r="I79" s="6"/>
+      <c r="I79" s="39"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="5"/>
-      <c r="I80" s="6"/>
+      <c r="I80" s="39"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="5"/>
-      <c r="I81" s="6"/>
+      <c r="I81" s="39"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="5"/>
-      <c r="I82" s="6"/>
+      <c r="I82" s="39"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="5"/>
-      <c r="I83" s="6"/>
+      <c r="I83" s="39"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="5"/>
-      <c r="I84" s="6"/>
+      <c r="I84" s="39"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="5"/>
-      <c r="I85" s="6"/>
+      <c r="I85" s="39"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
-      <c r="I86" s="6"/>
+      <c r="I86" s="39"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
-      <c r="I87" s="6"/>
+      <c r="I87" s="39"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
-      <c r="I88" s="6"/>
+      <c r="I88" s="39"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
-      <c r="I89" s="6"/>
+      <c r="I89" s="39"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
-      <c r="I90" s="6"/>
+      <c r="I90" s="39"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
-      <c r="I91" s="6"/>
+      <c r="I91" s="39"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
-      <c r="I92" s="6"/>
+      <c r="I92" s="39"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="5"/>
-      <c r="I93" s="6"/>
+      <c r="I93" s="39"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="5"/>
-      <c r="I94" s="6"/>
+      <c r="I94" s="39"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
-      <c r="I95" s="6"/>
+      <c r="I95" s="39"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="5"/>
-      <c r="I96" s="6"/>
+      <c r="I96" s="39"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="5"/>
-      <c r="I97" s="6"/>
+      <c r="I97" s="39"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="5"/>
-      <c r="I98" s="6"/>
+      <c r="I98" s="39"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="5"/>
-      <c r="I99" s="6"/>
+      <c r="I99" s="39"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="5"/>
-      <c r="I100" s="6"/>
+      <c r="I100" s="39"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
-      <c r="I101" s="6"/>
+      <c r="I101" s="39"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="5"/>
-      <c r="I102" s="6"/>
+      <c r="I102" s="39"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
-      <c r="I103" s="6"/>
+      <c r="I103" s="39"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
-      <c r="I104" s="6"/>
+      <c r="I104" s="39"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="5"/>
-      <c r="I105" s="6"/>
+      <c r="I105" s="39"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="5"/>
-      <c r="I106" s="6"/>
+      <c r="I106" s="39"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="5"/>
-      <c r="I107" s="6"/>
+      <c r="I107" s="39"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="5"/>
-      <c r="I108" s="6"/>
+      <c r="I108" s="39"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="5"/>
-      <c r="I109" s="6"/>
+      <c r="I109" s="39"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="5"/>
-      <c r="I110" s="6"/>
+      <c r="I110" s="39"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="5"/>
-      <c r="I111" s="6"/>
+      <c r="I111" s="39"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="5"/>
-      <c r="I112" s="6"/>
+      <c r="I112" s="39"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="5"/>
-      <c r="I113" s="6"/>
+      <c r="I113" s="39"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="5"/>
-      <c r="I114" s="6"/>
+      <c r="I114" s="39"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="5"/>
-      <c r="I115" s="6"/>
+      <c r="I115" s="39"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="5"/>
-      <c r="I116" s="6"/>
+      <c r="I116" s="39"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="5"/>
-      <c r="I117" s="6"/>
+      <c r="I117" s="39"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="5"/>
-      <c r="I118" s="6"/>
+      <c r="I118" s="39"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="5"/>
-      <c r="I119" s="6"/>
+      <c r="I119" s="39"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="5"/>
-      <c r="I120" s="6"/>
+      <c r="I120" s="39"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="5"/>
-      <c r="I121" s="6"/>
+      <c r="I121" s="39"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="5"/>
-      <c r="I122" s="6"/>
+      <c r="I122" s="39"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="5"/>
-      <c r="I123" s="6"/>
+      <c r="I123" s="39"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="5"/>
-      <c r="I124" s="6"/>
+      <c r="I124" s="39"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B125" s="5"/>
-      <c r="I125" s="6"/>
+      <c r="I125" s="39"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B126" s="5"/>
-      <c r="I126" s="6"/>
+      <c r="I126" s="39"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B127" s="5"/>
-      <c r="I127" s="6"/>
+      <c r="I127" s="39"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B128" s="5"/>
-      <c r="I128" s="6"/>
+      <c r="I128" s="39"/>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="5"/>
-      <c r="I129" s="6"/>
+      <c r="I129" s="39"/>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="5"/>
-      <c r="I130" s="6"/>
+      <c r="I130" s="39"/>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" s="5"/>
-      <c r="I131" s="6"/>
+      <c r="I131" s="39"/>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" s="5"/>
-      <c r="I132" s="6"/>
+      <c r="I132" s="39"/>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" s="5"/>
-      <c r="I133" s="6"/>
+      <c r="I133" s="39"/>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" s="5"/>
-      <c r="I134" s="6"/>
+      <c r="I134" s="39"/>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B135" s="5"/>
-      <c r="I135" s="6"/>
+      <c r="I135" s="39"/>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B136" s="5"/>
-      <c r="I136" s="6"/>
+      <c r="I136" s="39"/>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B137" s="5"/>
-      <c r="I137" s="6"/>
+      <c r="I137" s="39"/>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B138" s="5"/>
-      <c r="I138" s="6"/>
+      <c r="I138" s="39"/>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B139" s="5"/>
-      <c r="I139" s="6"/>
+      <c r="I139" s="39"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" s="5"/>
-      <c r="I140" s="6"/>
+      <c r="I140" s="39"/>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B141" s="5"/>
-      <c r="I141" s="6"/>
+      <c r="I141" s="39"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B142" s="5"/>
-      <c r="I142" s="6"/>
+      <c r="I142" s="39"/>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B143" s="5"/>
-      <c r="I143" s="6"/>
+      <c r="I143" s="39"/>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B144" s="5"/>
-      <c r="I144" s="6"/>
+      <c r="I144" s="39"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B145" s="5"/>
-      <c r="I145" s="6"/>
+      <c r="I145" s="39"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B146" s="5"/>
-      <c r="I146" s="6"/>
+      <c r="I146" s="39"/>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B147" s="5"/>
-      <c r="I147" s="6"/>
+      <c r="I147" s="39"/>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B148" s="5"/>
-      <c r="I148" s="6"/>
+      <c r="I148" s="39"/>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B149" s="5"/>
-      <c r="I149" s="6"/>
+      <c r="I149" s="39"/>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B150" s="5"/>
-      <c r="I150" s="6"/>
+      <c r="I150" s="39"/>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B151" s="5"/>
-      <c r="I151" s="6"/>
+      <c r="I151" s="39"/>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B152" s="5"/>
-      <c r="I152" s="6"/>
+      <c r="I152" s="39"/>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" s="5"/>
-      <c r="I153" s="6"/>
+      <c r="I153" s="39"/>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B154" s="5"/>
-      <c r="I154" s="6"/>
+      <c r="I154" s="39"/>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B155" s="5"/>
-      <c r="I155" s="6"/>
+      <c r="I155" s="39"/>
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B156" s="5"/>
-      <c r="I156" s="6"/>
+      <c r="I156" s="39"/>
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B157" s="5"/>
-      <c r="I157" s="6"/>
+      <c r="I157" s="39"/>
     </row>
     <row r="158" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B158" s="5"/>
-      <c r="I158" s="6"/>
+      <c r="I158" s="39"/>
     </row>
     <row r="159" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B159" s="5"/>
-      <c r="I159" s="6"/>
+      <c r="I159" s="39"/>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B160" s="5"/>
-      <c r="I160" s="6"/>
+      <c r="I160" s="39"/>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" s="5"/>
-      <c r="I161" s="6"/>
+      <c r="I161" s="39"/>
     </row>
     <row r="162" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B162" s="5"/>
-      <c r="I162" s="6"/>
+      <c r="I162" s="39"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" s="5"/>
-      <c r="I163" s="6"/>
+      <c r="I163" s="39"/>
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B164" s="5"/>
-      <c r="I164" s="6"/>
+      <c r="I164" s="39"/>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" s="5"/>
-      <c r="I165" s="6"/>
+      <c r="I165" s="39"/>
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B166" s="5"/>
-      <c r="I166" s="6"/>
+      <c r="I166" s="39"/>
     </row>
     <row r="167" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B167" s="5"/>
-      <c r="I167" s="6"/>
+      <c r="I167" s="39"/>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B168" s="5"/>
-      <c r="I168" s="6"/>
+      <c r="I168" s="39"/>
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B169" s="5"/>
-      <c r="I169" s="6"/>
+      <c r="I169" s="39"/>
     </row>
     <row r="170" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B170" s="5"/>
-      <c r="I170" s="6"/>
+      <c r="I170" s="39"/>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B171" s="5"/>
-      <c r="I171" s="6"/>
+      <c r="I171" s="39"/>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B172" s="5"/>
-      <c r="I172" s="6"/>
+      <c r="I172" s="39"/>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B173" s="5"/>
-      <c r="I173" s="6"/>
+      <c r="I173" s="39"/>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B174" s="5"/>
-      <c r="I174" s="6"/>
+      <c r="I174" s="39"/>
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B175" s="5"/>
-      <c r="I175" s="6"/>
+      <c r="I175" s="39"/>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B176" s="5"/>
-      <c r="I176" s="6"/>
+      <c r="I176" s="39"/>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" s="5"/>
-      <c r="I177" s="6"/>
+      <c r="I177" s="39"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" s="5"/>
-      <c r="I178" s="6"/>
+      <c r="I178" s="39"/>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B179" s="5"/>
-      <c r="I179" s="6"/>
+      <c r="I179" s="39"/>
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="5"/>
-      <c r="I180" s="6"/>
+      <c r="I180" s="39"/>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B181" s="5"/>
-      <c r="I181" s="6"/>
+      <c r="I181" s="39"/>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182" s="5"/>
-      <c r="I182" s="6"/>
+      <c r="I182" s="39"/>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B183" s="5"/>
-      <c r="I183" s="6"/>
+      <c r="I183" s="39"/>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B184" s="5"/>
-      <c r="I184" s="6"/>
+      <c r="I184" s="39"/>
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B185" s="5"/>
-      <c r="I185" s="6"/>
+      <c r="I185" s="39"/>
     </row>
     <row r="186" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B186" s="5"/>
-      <c r="I186" s="6"/>
+      <c r="I186" s="39"/>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B187" s="5"/>
-      <c r="I187" s="6"/>
+      <c r="I187" s="39"/>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B188" s="5"/>
-      <c r="I188" s="6"/>
+      <c r="I188" s="39"/>
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="5"/>
-      <c r="I189" s="6"/>
+      <c r="I189" s="39"/>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190" s="5"/>
-      <c r="I190" s="6"/>
+      <c r="I190" s="39"/>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B191" s="5"/>
-      <c r="I191" s="6"/>
+      <c r="I191" s="39"/>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B192" s="5"/>
-      <c r="I192" s="6"/>
+      <c r="I192" s="39"/>
     </row>
     <row r="193" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B193" s="5"/>
-      <c r="I193" s="6"/>
+      <c r="I193" s="39"/>
     </row>
     <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B194" s="5"/>
-      <c r="I194" s="6"/>
+      <c r="I194" s="39"/>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B195" s="5"/>
-      <c r="I195" s="6"/>
+      <c r="I195" s="39"/>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" s="5"/>
-      <c r="I196" s="6"/>
+      <c r="I196" s="39"/>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" s="5"/>
-      <c r="I197" s="6"/>
+      <c r="I197" s="39"/>
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B198" s="5"/>
-      <c r="I198" s="6"/>
+      <c r="I198" s="39"/>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" s="5"/>
-      <c r="I199" s="6"/>
+      <c r="I199" s="39"/>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B200" s="5"/>
-      <c r="I200" s="6"/>
+      <c r="I200" s="39"/>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B201" s="5"/>
-      <c r="I201" s="6"/>
+      <c r="I201" s="39"/>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B202" s="5"/>
-      <c r="I202" s="6"/>
+      <c r="I202" s="39"/>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B203" s="5"/>
-      <c r="I203" s="6"/>
+      <c r="I203" s="39"/>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B204" s="5"/>
-      <c r="I204" s="6"/>
+      <c r="I204" s="39"/>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B205" s="5"/>
-      <c r="I205" s="6"/>
+      <c r="I205" s="39"/>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B206" s="5"/>
-      <c r="I206" s="6"/>
+      <c r="I206" s="39"/>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" s="5"/>
-      <c r="I207" s="6"/>
+      <c r="I207" s="39"/>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B208" s="5"/>
-      <c r="I208" s="6"/>
+      <c r="I208" s="39"/>
     </row>
     <row r="209" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B209" s="5"/>
-      <c r="I209" s="6"/>
+      <c r="I209" s="39"/>
     </row>
     <row r="210" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B210" s="5"/>
-      <c r="I210" s="6"/>
+      <c r="I210" s="39"/>
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B211" s="5"/>
-      <c r="I211" s="6"/>
+      <c r="I211" s="39"/>
     </row>
     <row r="212" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B212" s="5"/>
-      <c r="I212" s="6"/>
+      <c r="I212" s="39"/>
     </row>
     <row r="213" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B213" s="5"/>
-      <c r="I213" s="6"/>
+      <c r="I213" s="39"/>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B214" s="5"/>
-      <c r="I214" s="6"/>
+      <c r="I214" s="39"/>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B215" s="5"/>
-      <c r="I215" s="6"/>
+      <c r="I215" s="39"/>
     </row>
     <row r="216" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B216" s="5"/>
-      <c r="I216" s="6"/>
+      <c r="I216" s="39"/>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B217" s="5"/>
-      <c r="I217" s="6"/>
+      <c r="I217" s="39"/>
     </row>
     <row r="218" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B218" s="5"/>
-      <c r="I218" s="6"/>
+      <c r="I218" s="39"/>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B219" s="5"/>
-      <c r="I219" s="6"/>
+      <c r="I219" s="39"/>
     </row>
     <row r="220" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B220" s="5"/>
-      <c r="I220" s="6"/>
+      <c r="I220" s="39"/>
     </row>
     <row r="221" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B221" s="5"/>
-      <c r="I221" s="6"/>
+      <c r="I221" s="39"/>
     </row>
     <row r="222" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B222" s="5"/>
-      <c r="I222" s="6"/>
+      <c r="I222" s="39"/>
     </row>
     <row r="223" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B223" s="5"/>
-      <c r="I223" s="6"/>
+      <c r="I223" s="39"/>
     </row>
     <row r="224" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B224" s="5"/>
-      <c r="I224" s="6"/>
+      <c r="I224" s="39"/>
     </row>
     <row r="225" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B225" s="5"/>
-      <c r="I225" s="6"/>
+      <c r="I225" s="39"/>
     </row>
     <row r="226" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B226" s="5"/>
-      <c r="I226" s="6"/>
+      <c r="I226" s="39"/>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B227" s="5"/>
-      <c r="I227" s="6"/>
+      <c r="I227" s="39"/>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B228" s="5"/>
-      <c r="I228" s="6"/>
+      <c r="I228" s="39"/>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B229" s="5"/>
-      <c r="I229" s="6"/>
+      <c r="I229" s="39"/>
     </row>
     <row r="230" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B230" s="5"/>
-      <c r="I230" s="6"/>
+      <c r="I230" s="39"/>
     </row>
     <row r="231" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B231" s="5"/>
-      <c r="I231" s="6"/>
+      <c r="I231" s="39"/>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B232" s="5"/>
-      <c r="I232" s="6"/>
+      <c r="I232" s="39"/>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B233" s="5"/>
-      <c r="I233" s="6"/>
+      <c r="I233" s="39"/>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B234" s="5"/>
-      <c r="I234" s="6"/>
+      <c r="I234" s="39"/>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B235" s="5"/>
-      <c r="I235" s="6"/>
+      <c r="I235" s="39"/>
     </row>
     <row r="236" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B236" s="5"/>
-      <c r="I236" s="6"/>
+      <c r="I236" s="39"/>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B237" s="5"/>
-      <c r="I237" s="6"/>
+      <c r="I237" s="39"/>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B238" s="5"/>
-      <c r="I238" s="6"/>
+      <c r="I238" s="39"/>
     </row>
     <row r="239" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B239" s="5"/>
-      <c r="I239" s="6"/>
+      <c r="I239" s="39"/>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B240" s="5"/>
-      <c r="I240" s="6"/>
+      <c r="I240" s="39"/>
     </row>
     <row r="241" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B241" s="5"/>
-      <c r="I241" s="6"/>
+      <c r="I241" s="39"/>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B242" s="5"/>
-      <c r="I242" s="6"/>
+      <c r="I242" s="39"/>
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B243" s="5"/>
-      <c r="I243" s="6"/>
+      <c r="I243" s="39"/>
     </row>
     <row r="244" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B244" s="5"/>
-      <c r="I244" s="6"/>
+      <c r="I244" s="39"/>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B245" s="5"/>
-      <c r="I245" s="6"/>
+      <c r="I245" s="39"/>
     </row>
     <row r="246" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B246" s="5"/>
-      <c r="I246" s="6"/>
+      <c r="I246" s="39"/>
     </row>
     <row r="247" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B247" s="5"/>
-      <c r="I247" s="6"/>
+      <c r="I247" s="39"/>
     </row>
     <row r="248" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B248" s="5"/>
-      <c r="I248" s="6"/>
+      <c r="I248" s="39"/>
     </row>
     <row r="249" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B249" s="5"/>
-      <c r="I249" s="6"/>
+      <c r="I249" s="39"/>
     </row>
     <row r="250" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B250" s="5"/>
-      <c r="I250" s="6"/>
+      <c r="I250" s="39"/>
     </row>
     <row r="251" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B251" s="5"/>
-      <c r="I251" s="6"/>
+      <c r="I251" s="39"/>
     </row>
     <row r="252" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B252" s="5"/>
-      <c r="I252" s="6"/>
+      <c r="I252" s="39"/>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B253" s="5"/>
-      <c r="I253" s="6"/>
+      <c r="I253" s="39"/>
     </row>
     <row r="254" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B254" s="5"/>
-      <c r="I254" s="6"/>
+      <c r="I254" s="39"/>
     </row>
     <row r="255" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B255" s="5"/>
-      <c r="I255" s="6"/>
+      <c r="I255" s="39"/>
     </row>
     <row r="256" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B256" s="5"/>
-      <c r="I256" s="6"/>
+      <c r="I256" s="39"/>
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B257" s="5"/>
-      <c r="I257" s="6"/>
+      <c r="I257" s="39"/>
     </row>
     <row r="258" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B258" s="5"/>
-      <c r="I258" s="6"/>
+      <c r="I258" s="39"/>
     </row>
     <row r="259" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B259" s="5"/>
-      <c r="I259" s="6"/>
+      <c r="I259" s="39"/>
     </row>
     <row r="260" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B260" s="5"/>
-      <c r="I260" s="6"/>
+      <c r="I260" s="39"/>
     </row>
     <row r="261" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B261" s="5"/>
-      <c r="I261" s="6"/>
+      <c r="I261" s="39"/>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B262" s="5"/>
-      <c r="I262" s="6"/>
+      <c r="I262" s="39"/>
     </row>
     <row r="263" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B263" s="5"/>
-      <c r="I263" s="6"/>
+      <c r="I263" s="39"/>
     </row>
     <row r="264" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B264" s="5"/>
-      <c r="I264" s="6"/>
+      <c r="I264" s="39"/>
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B265" s="5"/>
-      <c r="I265" s="6"/>
+      <c r="I265" s="39"/>
     </row>
     <row r="266" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B266" s="5"/>
-      <c r="I266" s="6"/>
+      <c r="I266" s="39"/>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B267" s="5"/>
-      <c r="I267" s="6"/>
+      <c r="I267" s="39"/>
     </row>
     <row r="268" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B268" s="5"/>
-      <c r="I268" s="6"/>
+      <c r="I268" s="39"/>
     </row>
     <row r="269" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B269" s="5"/>
-      <c r="I269" s="6"/>
+      <c r="I269" s="39"/>
     </row>
     <row r="270" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B270" s="5"/>
-      <c r="I270" s="6"/>
+      <c r="I270" s="39"/>
     </row>
     <row r="271" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B271" s="5"/>
-      <c r="I271" s="6"/>
+      <c r="I271" s="39"/>
     </row>
     <row r="272" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B272" s="5"/>
-      <c r="I272" s="6"/>
+      <c r="I272" s="39"/>
     </row>
     <row r="273" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B273" s="5"/>
-      <c r="I273" s="6"/>
+      <c r="I273" s="39"/>
     </row>
     <row r="274" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B274" s="5"/>
-      <c r="I274" s="6"/>
+      <c r="I274" s="39"/>
     </row>
     <row r="275" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B275" s="5"/>
-      <c r="I275" s="6"/>
+      <c r="I275" s="39"/>
     </row>
     <row r="276" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B276" s="5"/>
-      <c r="I276" s="6"/>
+      <c r="I276" s="39"/>
     </row>
     <row r="277" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B277" s="5"/>
-      <c r="I277" s="6"/>
+      <c r="I277" s="39"/>
     </row>
     <row r="278" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B278" s="5"/>
-      <c r="I278" s="6"/>
+      <c r="I278" s="39"/>
     </row>
     <row r="279" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B279" s="5"/>
-      <c r="I279" s="6"/>
+      <c r="I279" s="39"/>
     </row>
     <row r="280" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B280" s="5"/>
-      <c r="I280" s="6"/>
+      <c r="I280" s="39"/>
     </row>
     <row r="281" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B281" s="5"/>
-      <c r="I281" s="6"/>
+      <c r="I281" s="39"/>
     </row>
     <row r="282" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B282" s="5"/>
-      <c r="I282" s="6"/>
+      <c r="I282" s="39"/>
     </row>
     <row r="283" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B283" s="5"/>
-      <c r="I283" s="6"/>
+      <c r="I283" s="39"/>
     </row>
     <row r="284" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B284" s="5"/>
-      <c r="I284" s="6"/>
+      <c r="I284" s="39"/>
     </row>
     <row r="285" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B285" s="5"/>
-      <c r="I285" s="6"/>
+      <c r="I285" s="39"/>
     </row>
     <row r="286" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B286" s="5"/>
-      <c r="I286" s="6"/>
+      <c r="I286" s="39"/>
     </row>
     <row r="287" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B287" s="5"/>
-      <c r="I287" s="6"/>
+      <c r="I287" s="39"/>
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B288" s="5"/>
-      <c r="I288" s="6"/>
+      <c r="I288" s="39"/>
     </row>
     <row r="289" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B289" s="5"/>
-      <c r="I289" s="6"/>
+      <c r="I289" s="39"/>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B290" s="5"/>
-      <c r="I290" s="6"/>
+      <c r="I290" s="39"/>
     </row>
     <row r="291" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B291" s="5"/>
-      <c r="I291" s="6"/>
+      <c r="I291" s="39"/>
     </row>
     <row r="292" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B292" s="5"/>
-      <c r="I292" s="6"/>
+      <c r="I292" s="39"/>
     </row>
     <row r="293" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B293" s="5"/>
-      <c r="I293" s="6"/>
+      <c r="I293" s="39"/>
     </row>
     <row r="294" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B294" s="5"/>
-      <c r="I294" s="6"/>
+      <c r="I294" s="39"/>
     </row>
     <row r="295" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B295" s="5"/>
-      <c r="I295" s="6"/>
+      <c r="I295" s="39"/>
     </row>
     <row r="296" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B296" s="5"/>
-      <c r="I296" s="6"/>
+      <c r="I296" s="39"/>
     </row>
     <row r="297" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B297" s="5"/>
-      <c r="I297" s="6"/>
+      <c r="I297" s="39"/>
     </row>
     <row r="298" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B298" s="5"/>
-      <c r="I298" s="6"/>
+      <c r="I298" s="39"/>
     </row>
     <row r="299" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B299" s="5"/>
-      <c r="I299" s="6"/>
+      <c r="I299" s="39"/>
     </row>
     <row r="300" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B300" s="5"/>
-      <c r="I300" s="6"/>
+      <c r="I300" s="39"/>
     </row>
     <row r="301" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B301" s="5"/>
-      <c r="I301" s="6"/>
+      <c r="I301" s="39"/>
     </row>
     <row r="302" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B302" s="5"/>
-      <c r="I302" s="6"/>
+      <c r="I302" s="39"/>
     </row>
     <row r="303" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B303" s="5"/>
-      <c r="I303" s="6"/>
+      <c r="I303" s="39"/>
     </row>
     <row r="304" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B304" s="5"/>
-      <c r="I304" s="6"/>
+      <c r="I304" s="39"/>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B305" s="5"/>
-      <c r="I305" s="6"/>
+      <c r="I305" s="39"/>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B306" s="5"/>
-      <c r="I306" s="6"/>
+      <c r="I306" s="39"/>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B307" s="5"/>
-      <c r="I307" s="6"/>
+      <c r="I307" s="39"/>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B308" s="5"/>
-      <c r="I308" s="6"/>
+      <c r="I308" s="39"/>
     </row>
     <row r="309" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B309" s="5"/>
-      <c r="I309" s="6"/>
+      <c r="I309" s="39"/>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B310" s="5"/>
-      <c r="I310" s="6"/>
+      <c r="I310" s="39"/>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B311" s="5"/>
-      <c r="I311" s="6"/>
+      <c r="I311" s="39"/>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B312" s="5"/>
-      <c r="I312" s="6"/>
+      <c r="I312" s="39"/>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B313" s="5"/>
-      <c r="I313" s="6"/>
+      <c r="I313" s="39"/>
     </row>
     <row r="314" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B314" s="5"/>
-      <c r="I314" s="6"/>
+      <c r="I314" s="39"/>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B315" s="5"/>
-      <c r="I315" s="6"/>
+      <c r="I315" s="39"/>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B316" s="5"/>
-      <c r="I316" s="6"/>
+      <c r="I316" s="39"/>
     </row>
     <row r="317" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B317" s="5"/>
-      <c r="I317" s="6"/>
+      <c r="I317" s="39"/>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B318" s="5"/>
-      <c r="I318" s="6"/>
+      <c r="I318" s="39"/>
     </row>
     <row r="319" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B319" s="5"/>
-      <c r="I319" s="6"/>
+      <c r="I319" s="39"/>
     </row>
     <row r="320" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B320" s="5"/>
-      <c r="I320" s="6"/>
+      <c r="I320" s="39"/>
     </row>
     <row r="321" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B321" s="5"/>
-      <c r="I321" s="6"/>
+      <c r="I321" s="39"/>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B322" s="5"/>
-      <c r="I322" s="6"/>
+      <c r="I322" s="39"/>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B323" s="5"/>
-      <c r="I323" s="6"/>
+      <c r="I323" s="39"/>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B324" s="5"/>
-      <c r="I324" s="6"/>
+      <c r="I324" s="39"/>
     </row>
     <row r="325" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B325" s="5"/>
-      <c r="I325" s="6"/>
+      <c r="I325" s="39"/>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B326" s="5"/>
-      <c r="I326" s="6"/>
+      <c r="I326" s="39"/>
     </row>
     <row r="327" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B327" s="5"/>
-      <c r="I327" s="6"/>
+      <c r="I327" s="39"/>
     </row>
     <row r="328" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B328" s="5"/>
-      <c r="I328" s="6"/>
+      <c r="I328" s="39"/>
     </row>
     <row r="329" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B329" s="5"/>
-      <c r="I329" s="6"/>
+      <c r="I329" s="39"/>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B330" s="5"/>
-      <c r="I330" s="6"/>
+      <c r="I330" s="39"/>
     </row>
     <row r="331" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B331" s="5"/>
-      <c r="I331" s="6"/>
+      <c r="I331" s="39"/>
     </row>
     <row r="332" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B332" s="5"/>
-      <c r="I332" s="6"/>
+      <c r="I332" s="39"/>
     </row>
     <row r="333" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B333" s="5"/>
-      <c r="I333" s="6"/>
+      <c r="I333" s="39"/>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B334" s="5"/>
-      <c r="I334" s="6"/>
+      <c r="I334" s="39"/>
     </row>
     <row r="335" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B335" s="5"/>
-      <c r="I335" s="6"/>
+      <c r="I335" s="39"/>
     </row>
     <row r="336" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B336" s="5"/>
-      <c r="I336" s="6"/>
+      <c r="I336" s="39"/>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B337" s="5"/>
-      <c r="I337" s="6"/>
+      <c r="I337" s="39"/>
     </row>
     <row r="338" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B338" s="5"/>
-      <c r="I338" s="6"/>
+      <c r="I338" s="39"/>
     </row>
     <row r="339" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B339" s="5"/>
-      <c r="I339" s="6"/>
+      <c r="I339" s="39"/>
     </row>
     <row r="340" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B340" s="5"/>
-      <c r="I340" s="6"/>
+      <c r="I340" s="39"/>
     </row>
     <row r="341" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B341" s="5"/>
-      <c r="I341" s="6"/>
+      <c r="I341" s="39"/>
     </row>
     <row r="342" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B342" s="5"/>
-      <c r="I342" s="6"/>
+      <c r="I342" s="39"/>
     </row>
     <row r="343" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B343" s="5"/>
-      <c r="I343" s="6"/>
+      <c r="I343" s="39"/>
     </row>
     <row r="344" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B344" s="5"/>
-      <c r="I344" s="6"/>
+      <c r="I344" s="39"/>
     </row>
     <row r="345" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B345" s="5"/>
-      <c r="I345" s="6"/>
+      <c r="I345" s="39"/>
     </row>
     <row r="346" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B346" s="5"/>
-      <c r="I346" s="6"/>
+      <c r="I346" s="39"/>
     </row>
     <row r="347" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B347" s="5"/>
-      <c r="I347" s="6"/>
+      <c r="I347" s="39"/>
     </row>
     <row r="348" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B348" s="5"/>
-      <c r="I348" s="6"/>
+      <c r="I348" s="39"/>
     </row>
     <row r="349" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B349" s="5"/>
-      <c r="I349" s="6"/>
+      <c r="I349" s="39"/>
     </row>
     <row r="350" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B350" s="5"/>
-      <c r="I350" s="6"/>
+      <c r="I350" s="39"/>
     </row>
     <row r="351" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B351" s="5"/>
-      <c r="I351" s="6"/>
+      <c r="I351" s="39"/>
     </row>
     <row r="352" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B352" s="5"/>
-      <c r="I352" s="6"/>
+      <c r="I352" s="39"/>
     </row>
     <row r="353" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B353" s="5"/>
-      <c r="I353" s="6"/>
+      <c r="I353" s="39"/>
     </row>
     <row r="354" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B354" s="5"/>
-      <c r="I354" s="6"/>
+      <c r="I354" s="39"/>
     </row>
     <row r="355" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B355" s="5"/>
-      <c r="I355" s="6"/>
+      <c r="I355" s="39"/>
     </row>
     <row r="356" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B356" s="5"/>
-      <c r="I356" s="6"/>
+      <c r="I356" s="39"/>
     </row>
     <row r="357" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B357" s="5"/>
-      <c r="I357" s="6"/>
+      <c r="I357" s="39"/>
     </row>
     <row r="358" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B358" s="5"/>
-      <c r="I358" s="6"/>
+      <c r="I358" s="39"/>
     </row>
     <row r="359" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B359" s="5"/>
-      <c r="I359" s="6"/>
+      <c r="I359" s="39"/>
     </row>
     <row r="360" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B360" s="5"/>
-      <c r="I360" s="6"/>
+      <c r="I360" s="39"/>
     </row>
     <row r="361" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B361" s="5"/>
-      <c r="I361" s="6"/>
+      <c r="I361" s="39"/>
     </row>
     <row r="362" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B362" s="5"/>
-      <c r="I362" s="6"/>
+      <c r="I362" s="39"/>
     </row>
     <row r="363" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B363" s="5"/>
-      <c r="I363" s="6"/>
+      <c r="I363" s="39"/>
     </row>
     <row r="364" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B364" s="5"/>
-      <c r="I364" s="6"/>
+      <c r="I364" s="39"/>
     </row>
     <row r="365" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B365" s="5"/>
-      <c r="I365" s="6"/>
+      <c r="I365" s="39"/>
     </row>
     <row r="366" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B366" s="5"/>
-      <c r="I366" s="6"/>
+      <c r="I366" s="39"/>
     </row>
     <row r="367" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B367" s="5"/>
-      <c r="I367" s="6"/>
+      <c r="I367" s="39"/>
     </row>
     <row r="368" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B368" s="5"/>
-      <c r="I368" s="6"/>
+      <c r="I368" s="39"/>
     </row>
     <row r="369" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B369" s="5"/>
-      <c r="I369" s="6"/>
+      <c r="I369" s="39"/>
     </row>
     <row r="370" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B370" s="5"/>
-      <c r="I370" s="6"/>
+      <c r="I370" s="39"/>
     </row>
     <row r="371" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B371" s="5"/>
-      <c r="I371" s="6"/>
+      <c r="I371" s="39"/>
     </row>
     <row r="372" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B372" s="5"/>
-      <c r="I372" s="6"/>
+      <c r="I372" s="39"/>
     </row>
     <row r="373" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B373" s="5"/>
-      <c r="I373" s="6"/>
+      <c r="I373" s="39"/>
     </row>
     <row r="374" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B374" s="5"/>
-      <c r="I374" s="6"/>
+      <c r="I374" s="39"/>
     </row>
     <row r="375" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B375" s="5"/>
-      <c r="I375" s="6"/>
+      <c r="I375" s="39"/>
     </row>
     <row r="376" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B376" s="5"/>
-      <c r="I376" s="6"/>
+      <c r="I376" s="39"/>
     </row>
     <row r="377" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B377" s="5"/>
-      <c r="I377" s="6"/>
+      <c r="I377" s="39"/>
     </row>
     <row r="378" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B378" s="5"/>
-      <c r="I378" s="6"/>
+      <c r="I378" s="39"/>
     </row>
     <row r="379" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B379" s="5"/>
-      <c r="I379" s="6"/>
+      <c r="I379" s="39"/>
     </row>
     <row r="380" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B380" s="5"/>
-      <c r="I380" s="6"/>
+      <c r="I380" s="39"/>
     </row>
     <row r="381" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B381" s="5"/>
-      <c r="I381" s="6"/>
+      <c r="I381" s="39"/>
     </row>
     <row r="382" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B382" s="5"/>
-      <c r="I382" s="6"/>
+      <c r="I382" s="39"/>
     </row>
     <row r="383" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B383" s="5"/>
-      <c r="I383" s="6"/>
+      <c r="I383" s="39"/>
     </row>
     <row r="384" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B384" s="5"/>
-      <c r="I384" s="6"/>
+      <c r="I384" s="39"/>
     </row>
     <row r="385" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B385" s="5"/>
-      <c r="I385" s="6"/>
+      <c r="I385" s="39"/>
     </row>
     <row r="386" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B386" s="5"/>
-      <c r="I386" s="6"/>
+      <c r="I386" s="39"/>
     </row>
     <row r="387" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B387" s="5"/>
-      <c r="I387" s="6"/>
+      <c r="I387" s="39"/>
     </row>
     <row r="388" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B388" s="5"/>
-      <c r="I388" s="6"/>
+      <c r="I388" s="39"/>
     </row>
     <row r="389" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B389" s="5"/>
-      <c r="I389" s="6"/>
+      <c r="I389" s="39"/>
     </row>
     <row r="390" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B390" s="5"/>
-      <c r="I390" s="6"/>
+      <c r="I390" s="39"/>
     </row>
     <row r="391" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B391" s="5"/>
-      <c r="I391" s="6"/>
+      <c r="I391" s="39"/>
     </row>
     <row r="392" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B392" s="5"/>
-      <c r="I392" s="6"/>
+      <c r="I392" s="39"/>
     </row>
     <row r="393" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B393" s="5"/>
-      <c r="I393" s="6"/>
+      <c r="I393" s="39"/>
     </row>
     <row r="394" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B394" s="5"/>
-      <c r="I394" s="6"/>
+      <c r="I394" s="39"/>
     </row>
     <row r="395" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B395" s="5"/>
-      <c r="I395" s="6"/>
+      <c r="I395" s="39"/>
     </row>
     <row r="396" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B396" s="5"/>
-      <c r="I396" s="6"/>
+      <c r="I396" s="39"/>
     </row>
     <row r="397" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B397" s="5"/>
-      <c r="I397" s="6"/>
+      <c r="I397" s="39"/>
     </row>
     <row r="398" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B398" s="5"/>
-      <c r="I398" s="6"/>
+      <c r="I398" s="39"/>
     </row>
     <row r="399" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B399" s="5"/>
-      <c r="I399" s="6"/>
+      <c r="I399" s="39"/>
     </row>
     <row r="400" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B400" s="5"/>
-      <c r="I400" s="6"/>
+      <c r="I400" s="39"/>
     </row>
     <row r="401" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B401" s="5"/>
-      <c r="I401" s="6"/>
+      <c r="I401" s="39"/>
     </row>
     <row r="402" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B402" s="5"/>
-      <c r="I402" s="6"/>
+      <c r="I402" s="39"/>
     </row>
     <row r="403" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B403" s="5"/>
-      <c r="I403" s="6"/>
+      <c r="I403" s="39"/>
     </row>
     <row r="404" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B404" s="5"/>
-      <c r="I404" s="6"/>
+      <c r="I404" s="39"/>
     </row>
     <row r="405" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B405" s="5"/>
-      <c r="I405" s="6"/>
+      <c r="I405" s="39"/>
     </row>
     <row r="406" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B406" s="5"/>
-      <c r="I406" s="6"/>
+      <c r="I406" s="39"/>
     </row>
     <row r="407" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B407" s="5"/>
-      <c r="I407" s="6"/>
+      <c r="I407" s="39"/>
     </row>
     <row r="408" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B408" s="5"/>
-      <c r="I408" s="6"/>
+      <c r="I408" s="39"/>
     </row>
     <row r="409" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B409" s="5"/>
-      <c r="I409" s="6"/>
+      <c r="I409" s="39"/>
     </row>
     <row r="410" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B410" s="5"/>
-      <c r="I410" s="6"/>
+      <c r="I410" s="39"/>
     </row>
     <row r="411" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B411" s="5"/>
-      <c r="I411" s="6"/>
+      <c r="I411" s="39"/>
     </row>
     <row r="412" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B412" s="5"/>
-      <c r="I412" s="6"/>
+      <c r="I412" s="39"/>
     </row>
     <row r="413" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B413" s="5"/>
-      <c r="I413" s="6"/>
+      <c r="I413" s="39"/>
     </row>
     <row r="414" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B414" s="5"/>
-      <c r="I414" s="6"/>
+      <c r="I414" s="39"/>
     </row>
     <row r="415" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B415" s="5"/>
-      <c r="I415" s="6"/>
+      <c r="I415" s="39"/>
     </row>
     <row r="416" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B416" s="5"/>
-      <c r="I416" s="6"/>
+      <c r="I416" s="39"/>
     </row>
     <row r="417" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B417" s="5"/>
-      <c r="I417" s="6"/>
+      <c r="I417" s="39"/>
     </row>
     <row r="418" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B418" s="5"/>
-      <c r="I418" s="6"/>
+      <c r="I418" s="39"/>
     </row>
     <row r="419" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B419" s="5"/>
-      <c r="I419" s="6"/>
+      <c r="I419" s="39"/>
     </row>
     <row r="420" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B420" s="5"/>
-      <c r="I420" s="6"/>
+      <c r="I420" s="39"/>
     </row>
     <row r="421" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B421" s="5"/>
-      <c r="I421" s="6"/>
+      <c r="I421" s="39"/>
     </row>
     <row r="422" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B422" s="5"/>
-      <c r="I422" s="6"/>
+      <c r="I422" s="39"/>
     </row>
     <row r="423" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B423" s="5"/>
-      <c r="I423" s="6"/>
+      <c r="I423" s="39"/>
     </row>
     <row r="424" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B424" s="5"/>
-      <c r="I424" s="6"/>
+      <c r="I424" s="39"/>
     </row>
     <row r="425" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B425" s="5"/>
-      <c r="I425" s="6"/>
+      <c r="I425" s="39"/>
     </row>
     <row r="426" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B426" s="5"/>
-      <c r="I426" s="6"/>
+      <c r="I426" s="39"/>
     </row>
     <row r="427" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B427" s="5"/>
-      <c r="I427" s="6"/>
+      <c r="I427" s="39"/>
     </row>
     <row r="428" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B428" s="5"/>
-      <c r="I428" s="6"/>
+      <c r="I428" s="39"/>
     </row>
     <row r="429" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B429" s="5"/>
-      <c r="I429" s="6"/>
+      <c r="I429" s="39"/>
     </row>
     <row r="430" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B430" s="5"/>
-      <c r="I430" s="6"/>
+      <c r="I430" s="39"/>
     </row>
     <row r="431" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B431" s="5"/>
-      <c r="I431" s="6"/>
+      <c r="I431" s="39"/>
     </row>
     <row r="432" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B432" s="5"/>
-      <c r="I432" s="6"/>
+      <c r="I432" s="39"/>
     </row>
     <row r="433" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B433" s="5"/>
-      <c r="I433" s="6"/>
+      <c r="I433" s="39"/>
     </row>
     <row r="434" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B434" s="5"/>
-      <c r="I434" s="6"/>
+      <c r="I434" s="39"/>
     </row>
     <row r="435" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B435" s="5"/>
-      <c r="I435" s="6"/>
+      <c r="I435" s="39"/>
     </row>
     <row r="436" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B436" s="5"/>
-      <c r="I436" s="6"/>
+      <c r="I436" s="39"/>
     </row>
     <row r="437" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B437" s="5"/>
-      <c r="I437" s="6"/>
+      <c r="I437" s="39"/>
     </row>
     <row r="438" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B438" s="5"/>
-      <c r="I438" s="6"/>
+      <c r="I438" s="39"/>
     </row>
     <row r="439" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B439" s="5"/>
-      <c r="I439" s="6"/>
+      <c r="I439" s="39"/>
     </row>
     <row r="440" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B440" s="5"/>
-      <c r="I440" s="6"/>
+      <c r="I440" s="39"/>
     </row>
     <row r="441" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B441" s="5"/>
-      <c r="I441" s="6"/>
+      <c r="I441" s="39"/>
     </row>
     <row r="442" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B442" s="5"/>
-      <c r="I442" s="6"/>
+      <c r="I442" s="39"/>
     </row>
     <row r="443" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B443" s="5"/>
-      <c r="I443" s="6"/>
+      <c r="I443" s="39"/>
     </row>
     <row r="444" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B444" s="5"/>
-      <c r="I444" s="6"/>
+      <c r="I444" s="39"/>
     </row>
     <row r="445" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B445" s="5"/>
-      <c r="I445" s="6"/>
+      <c r="I445" s="39"/>
     </row>
     <row r="446" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B446" s="5"/>
-      <c r="I446" s="6"/>
+      <c r="I446" s="39"/>
     </row>
     <row r="447" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B447" s="5"/>
-      <c r="I447" s="6"/>
+      <c r="I447" s="39"/>
     </row>
     <row r="448" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B448" s="5"/>
-      <c r="I448" s="6"/>
+      <c r="I448" s="39"/>
     </row>
     <row r="449" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B449" s="5"/>
-      <c r="I449" s="6"/>
+      <c r="I449" s="39"/>
     </row>
     <row r="450" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B450" s="5"/>
-      <c r="I450" s="6"/>
+      <c r="I450" s="39"/>
     </row>
     <row r="451" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B451" s="5"/>
-      <c r="I451" s="6"/>
+      <c r="I451" s="39"/>
     </row>
     <row r="452" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B452" s="5"/>
-      <c r="I452" s="6"/>
+      <c r="I452" s="39"/>
     </row>
     <row r="453" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B453" s="5"/>
-      <c r="I453" s="6"/>
+      <c r="I453" s="39"/>
     </row>
     <row r="454" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B454" s="5"/>
-      <c r="I454" s="6"/>
+      <c r="I454" s="39"/>
     </row>
     <row r="455" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B455" s="5"/>
-      <c r="I455" s="6"/>
+      <c r="I455" s="39"/>
     </row>
     <row r="456" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B456" s="12"/>
+      <c r="B456" s="11"/>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
-      <c r="E456" s="3"/>
+      <c r="E456" s="37"/>
       <c r="F456" s="3"/>
       <c r="G456" s="3"/>
       <c r="H456" s="3"/>
-      <c r="I456" s="13"/>
+      <c r="I456" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="M3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E248 E3:F7 I9:I288 I3:I7">
+  <conditionalFormatting sqref="E9:E248 E3:F4 E6:F8 E5 I3:I288">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>5</formula>
       <formula>7</formula>

</xml_diff>